<commit_message>
Desafio 5 - Nivel 3
</commit_message>
<xml_diff>
--- a/Desafio4/data/b3.xlsx
+++ b/Desafio4/data/b3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationEdge\Desafios\Desafio4\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71041CB3-AEB0-4D34-9298-1B8D3479E2AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66BA545-ABDD-4FAD-B266-76712A05E186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Magazine Luiza</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>VALE3:BVMF</t>
+  </si>
+  <si>
+    <t>Companhia Siderúrgica Nacional</t>
+  </si>
+  <si>
+    <t>CSNA3:BVMF</t>
+  </si>
+  <si>
+    <t>Eletrobras</t>
+  </si>
+  <si>
+    <t>ELET6:BVMF</t>
   </si>
 </sst>
 </file>
@@ -411,15 +423,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -463,6 +475,22 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>